<commit_message>
1000tk from Taher & his Brother
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE531CA-FA74-4E46-871A-B9EB93D3B634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177555F1-96B6-4EAB-BB65-38EEB1D6DE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1198,7 +1198,7 @@
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>375</v>
+        <v>625</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1302,7 +1302,7 @@
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>-125.00000000000001</v>
+        <v>625</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -2274,7 +2274,7 @@
       </c>
       <c r="AH24" s="4">
         <f>SUM(AG23:AG36)</f>
-        <v>885</v>
+        <v>1885</v>
       </c>
       <c r="AI24" s="4">
         <f>AG43</f>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="AJ24" s="4">
         <f>AH24-AI24</f>
-        <v>85</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2500,7 +2500,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="4"/>
-        <v>500</v>
+        <v>750</v>
       </c>
       <c r="AH27" s="4"/>
       <c r="AI27" s="4"/>
@@ -2603,7 +2603,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="1">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="AG28" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="AH28" s="4"/>
       <c r="AI28" s="4"/>

</xml_diff>

<commit_message>
Moyla correction & March 4&5
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E42F07-7006-414F-B6BD-D58A82FBBD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CCB005-A95A-4BE7-99CE-BEEFE6C30BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -709,8 +709,12 @@
       <c r="D3" s="1">
         <v>2.5</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.5</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -785,19 +789,19 @@
       </c>
       <c r="AG3" s="1">
         <f>SUM(B3:AF3)</f>
-        <v>7.5</v>
+        <v>11.5</v>
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>26.666666666666668</v>
+        <v>27.30263157894737</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>200</v>
+        <v>313.98026315789474</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>-214.28571400000001</v>
+        <v>-313.26597744360902</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -816,8 +820,12 @@
       <c r="D4" s="1">
         <v>2.5</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.5</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -892,16 +900,16 @@
       </c>
       <c r="AG4" s="1">
         <f>SUM(B4:AF4)</f>
-        <v>7.5</v>
+        <v>11.5</v>
       </c>
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>200</v>
+        <v>313.98026315789474</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>-214.28571400000001</v>
+        <v>-328.26597744360902</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -920,8 +928,12 @@
       <c r="D5" s="1">
         <v>0</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1001,11 +1013,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>66.666666666666671</v>
+        <v>68.256578947368425</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>-80.95238066666667</v>
+        <v>-82.542293233082717</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1024,8 +1036,12 @@
       <c r="D6" s="1">
         <v>2.5</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="E6" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.5</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1100,16 +1116,16 @@
       </c>
       <c r="AG6" s="1">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>200</v>
+        <v>341.28289473684214</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-214.28571400000001</v>
+        <v>-355.56860902255642</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1128,8 +1144,12 @@
       <c r="D7" s="1">
         <v>2.5</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2.5</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1204,16 +1224,16 @@
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>200</v>
+        <v>341.28289473684214</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>535.71428600000002</v>
+        <v>394.43139097744353</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1232,8 +1252,12 @@
       <c r="D8" s="1">
         <v>2.5</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="E8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.5</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1308,16 +1332,16 @@
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>12.5</v>
       </c>
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>200</v>
+        <v>341.28289473684214</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>535.71428600000002</v>
+        <v>394.43139097744353</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1336,8 +1360,12 @@
       <c r="D9" s="1">
         <v>2.5</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2.5</v>
+      </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1412,16 +1440,16 @@
       </c>
       <c r="AG9" s="1">
         <f>SUM(B9:AF9)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>213.33333333333334</v>
+        <v>354.93421052631584</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>157.38095266666667</v>
+        <v>15.780075187969885</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -1779,11 +1807,11 @@
       </c>
       <c r="E17" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="2"/>
@@ -1931,7 +1959,7 @@
       <c r="AF18" s="7"/>
       <c r="AG18" s="1">
         <f>SUM(AG3:AG16)</f>
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -2090,10 +2118,11 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1">
-        <v>-14.285714</v>
+        <f>-100/7</f>
+        <v>-14.285714285714286</v>
       </c>
       <c r="F23" s="1">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
@@ -2175,7 +2204,7 @@
       </c>
       <c r="AG23" s="1">
         <f t="shared" ref="AG23:AG36" si="3">SUM(B23:AF23)</f>
-        <v>-14.285714</v>
+        <v>0.71428571428571352</v>
       </c>
       <c r="AH23" s="1" t="s">
         <v>10</v>
@@ -2201,7 +2230,8 @@
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>-14.285714</v>
+        <f t="shared" ref="E24:E29" si="4">-100/7</f>
+        <v>-14.285714285714286</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -2286,19 +2316,19 @@
       </c>
       <c r="AG24" s="1">
         <f t="shared" si="3"/>
-        <v>-14.285714</v>
+        <v>-14.285714285714286</v>
       </c>
       <c r="AH24" s="6">
         <f>SUM(AG23:AG36)</f>
-        <v>1785.0000019999998</v>
+        <v>1800</v>
       </c>
       <c r="AI24" s="6">
         <f>AG43</f>
-        <v>800</v>
+        <v>1315</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>985.00000199999977</v>
+        <v>485</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2315,7 +2345,8 @@
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>-14.285714</v>
+        <f t="shared" si="4"/>
+        <v>-14.285714285714286</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1">
@@ -2398,7 +2429,7 @@
       </c>
       <c r="AG25" s="1">
         <f t="shared" si="3"/>
-        <v>-14.285714</v>
+        <v>-14.285714285714286</v>
       </c>
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
@@ -2416,7 +2447,8 @@
         <v>0</v>
       </c>
       <c r="E26" s="1">
-        <v>-14.285714</v>
+        <f t="shared" si="4"/>
+        <v>-14.285714285714286</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -2501,7 +2533,7 @@
       </c>
       <c r="AG26" s="1">
         <f t="shared" si="3"/>
-        <v>-14.285714</v>
+        <v>-14.285714285714286</v>
       </c>
       <c r="AH26" s="6"/>
       <c r="AI26" s="6"/>
@@ -2519,7 +2551,8 @@
         <v>250</v>
       </c>
       <c r="E27" s="1">
-        <v>-14.285714</v>
+        <f t="shared" si="4"/>
+        <v>-14.285714285714286</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -2604,7 +2637,7 @@
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="3"/>
-        <v>735.71428600000002</v>
+        <v>735.71428571428567</v>
       </c>
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
@@ -2622,7 +2655,8 @@
         <v>750</v>
       </c>
       <c r="E28" s="1">
-        <v>-14.285714</v>
+        <f t="shared" si="4"/>
+        <v>-14.285714285714286</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -2707,7 +2741,7 @@
       </c>
       <c r="AG28" s="1">
         <f t="shared" si="3"/>
-        <v>735.71428600000002</v>
+        <v>735.71428571428567</v>
       </c>
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>
@@ -2727,7 +2761,8 @@
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>-14.285714</v>
+        <f t="shared" si="4"/>
+        <v>-14.285714285714286</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -2812,7 +2847,7 @@
       </c>
       <c r="AG29" s="1">
         <f t="shared" si="3"/>
-        <v>370.71428600000002</v>
+        <v>370.71428571428572</v>
       </c>
       <c r="AH29" s="6"/>
       <c r="AI29" s="6"/>
@@ -3300,7 +3335,9 @@
         <v>415</v>
       </c>
       <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="E43" s="1">
+        <v>515</v>
+      </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -3376,7 +3413,7 @@
       </c>
       <c r="AG43" s="1">
         <f>SUM(B43:AF43)</f>
-        <v>800</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3388,128 +3425,128 @@
         <v>175</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" ref="C44:AF44" si="4">C17*0.2*50</f>
+        <f t="shared" ref="C44:AF44" si="5">C17*0.2*50</f>
         <v>155</v>
       </c>
       <c r="D44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>150</v>
       </c>
       <c r="F44" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>130</v>
       </c>
       <c r="G44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AD44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AF44" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AG44" s="5">
         <f>SUM(B44:AF44)</f>
-        <v>480</v>
+        <v>760</v>
       </c>
     </row>
     <row r="45" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3522,128 +3559,128 @@
         <v>560</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" ref="C46:AF46" si="5">SUM(C43+C44)</f>
+        <f t="shared" ref="C46:AF46" si="6">SUM(C43+C44)</f>
         <v>570</v>
       </c>
       <c r="D46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="E46" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>665</v>
       </c>
       <c r="F46" s="5">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>130</v>
       </c>
       <c r="G46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="M46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="P46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="R46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="T46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="W46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="X46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Y46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Z46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AA46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AC46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AD46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AE46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AF46" s="5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>1280</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Nayem -230 & Mahfuz +500
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CCB005-A95A-4BE7-99CE-BEEFE6C30BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500AEBB2-27B3-4434-9658-C6551F87BD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -909,7 +909,7 @@
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>-328.26597744360902</v>
+        <v>171.73402255639098</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>15.780075187969885</v>
+        <v>-214.21992481203011</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -2234,7 +2234,7 @@
         <v>-14.285714285714286</v>
       </c>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
@@ -2316,11 +2316,11 @@
       </c>
       <c r="AG24" s="1">
         <f t="shared" si="3"/>
-        <v>-14.285714285714286</v>
+        <v>485.71428571428572</v>
       </c>
       <c r="AH24" s="6">
         <f>SUM(AG23:AG36)</f>
-        <v>1800</v>
+        <v>2070</v>
       </c>
       <c r="AI24" s="6">
         <f>AG43</f>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>485</v>
+        <v>755</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2765,7 +2765,7 @@
         <v>-14.285714285714286</v>
       </c>
       <c r="F29" s="1">
-        <v>0</v>
+        <v>-230</v>
       </c>
       <c r="G29" s="1">
         <v>0</v>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="AG29" s="1">
         <f t="shared" si="3"/>
-        <v>370.71428571428572</v>
+        <v>140.71428571428572</v>
       </c>
       <c r="AH29" s="6"/>
       <c r="AI29" s="6"/>

</xml_diff>

<commit_message>
Rakib +1000, Rakib Extra meal, Bazar 11, Nayem +11
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500AEBB2-27B3-4434-9658-C6551F87BD33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113DD605-FD4F-418B-BD5A-1F2130733EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>meal rate</t>
   </si>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -713,7 +713,7 @@
         <v>2.5</v>
       </c>
       <c r="F3" s="1">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -789,19 +789,19 @@
       </c>
       <c r="AG3" s="1">
         <f>SUM(B3:AF3)</f>
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>27.30263157894737</v>
+        <v>27.220779220779221</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>313.98026315789474</v>
+        <v>340.25974025974028</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>-313.26597744360902</v>
+        <v>660.45454545454538</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -905,11 +905,11 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>313.98026315789474</v>
+        <v>313.03896103896102</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>171.73402255639098</v>
+        <v>172.6753246753247</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1013,11 +1013,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>68.256578947368425</v>
+        <v>68.051948051948045</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>-82.542293233082717</v>
+        <v>-82.337662337662337</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1121,11 +1121,11 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>341.28289473684214</v>
+        <v>340.25974025974028</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-355.56860902255642</v>
+        <v>-354.54545454545456</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1229,11 +1229,11 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>341.28289473684214</v>
+        <v>340.25974025974028</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>394.43139097744353</v>
+        <v>395.45454545454538</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1337,11 +1337,11 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>341.28289473684214</v>
+        <v>340.25974025974028</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>394.43139097744353</v>
+        <v>395.45454545454538</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1445,11 +1445,11 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>354.93421052631584</v>
+        <v>353.87012987012986</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-214.21992481203011</v>
+        <v>-202.15584415584414</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="2"/>
@@ -1959,7 +1959,7 @@
       <c r="AF18" s="7"/>
       <c r="AG18" s="1">
         <f>SUM(AG3:AG16)</f>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -2125,7 +2125,7 @@
         <v>15</v>
       </c>
       <c r="G23" s="1">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
@@ -2204,7 +2204,7 @@
       </c>
       <c r="AG23" s="1">
         <f t="shared" ref="AG23:AG36" si="3">SUM(B23:AF23)</f>
-        <v>0.71428571428571352</v>
+        <v>1000.7142857142857</v>
       </c>
       <c r="AH23" s="1" t="s">
         <v>10</v>
@@ -2320,15 +2320,15 @@
       </c>
       <c r="AH24" s="6">
         <f>SUM(AG23:AG36)</f>
-        <v>2070</v>
+        <v>3081</v>
       </c>
       <c r="AI24" s="6">
         <f>AG43</f>
-        <v>1315</v>
+        <v>1326</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>755</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2768,7 +2768,7 @@
         <v>-230</v>
       </c>
       <c r="G29" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H29" s="1">
         <v>0</v>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="AG29" s="1">
         <f t="shared" si="3"/>
-        <v>140.71428571428572</v>
+        <v>151.71428571428572</v>
       </c>
       <c r="AH29" s="6"/>
       <c r="AI29" s="6"/>
@@ -3295,7 +3295,9 @@
       <c r="E42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -3338,7 +3340,9 @@
       <c r="E43" s="1">
         <v>515</v>
       </c>
-      <c r="F43" s="1"/>
+      <c r="F43" s="1">
+        <v>11</v>
+      </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -3413,7 +3417,7 @@
       </c>
       <c r="AG43" s="1">
         <f>SUM(B43:AF43)</f>
-        <v>1315</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3438,7 +3442,7 @@
       </c>
       <c r="F44" s="5">
         <f t="shared" si="5"/>
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="G44" s="5">
         <f t="shared" si="5"/>
@@ -3546,7 +3550,7 @@
       </c>
       <c r="AG44" s="5">
         <f>SUM(B44:AF44)</f>
-        <v>760</v>
+        <v>770</v>
       </c>
     </row>
     <row r="45" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3572,7 +3576,7 @@
       </c>
       <c r="F46" s="5">
         <f t="shared" si="6"/>
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="G46" s="5">
         <f t="shared" si="6"/>
@@ -3680,7 +3684,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>2075</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minhaz +45, Bazar -545
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EE16E7-465B-4E25-BB37-DF4BAF753FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5156AC-BA4F-4A1F-B0C9-F020B03698E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>meal rate</t>
   </si>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -715,9 +715,15 @@
       <c r="F3" s="1">
         <v>2.5</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
       <c r="J3" s="1">
         <v>0</v>
       </c>
@@ -793,15 +799,15 @@
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>27.415584415584416</v>
+        <v>29.443298969072163</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>342.69480519480521</v>
+        <v>368.04123711340202</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>658.01948051948045</v>
+        <v>632.6730486008837</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -826,9 +832,15 @@
       <c r="F4" s="1">
         <v>1.5</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
       <c r="J4" s="1">
         <v>0</v>
       </c>
@@ -905,11 +917,11 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>315.27922077922079</v>
+        <v>338.59793814432987</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>170.43506493506493</v>
+        <v>147.11634756995585</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -934,9 +946,15 @@
       <c r="F5" s="1">
         <v>0</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
       <c r="J5" s="1">
         <v>0</v>
       </c>
@@ -1013,11 +1031,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>68.538961038961034</v>
+        <v>73.608247422680407</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>-82.824675324675326</v>
+        <v>-87.893961708394698</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1042,8 +1060,12 @@
       <c r="F6" s="1">
         <v>2.5</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2.5</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1">
         <v>0</v>
@@ -1116,16 +1138,16 @@
       </c>
       <c r="AG6" s="1">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>17.5</v>
       </c>
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>342.69480519480521</v>
+        <v>515.25773195876286</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-356.98051948051949</v>
+        <v>-484.54344624447714</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1150,8 +1172,12 @@
       <c r="F7" s="1">
         <v>2.5</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H7" s="1">
+        <v>2.5</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1">
         <v>0</v>
@@ -1224,16 +1250,16 @@
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>17.5</v>
       </c>
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>342.69480519480521</v>
+        <v>515.25773195876286</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>393.01948051948045</v>
+        <v>220.4565537555228</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1258,8 +1284,12 @@
       <c r="F8" s="1">
         <v>2.5</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2.5</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1">
         <v>0</v>
@@ -1332,16 +1362,16 @@
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>17.5</v>
       </c>
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>342.69480519480521</v>
+        <v>515.25773195876286</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>393.01948051948045</v>
+        <v>220.4565537555228</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1366,8 +1396,12 @@
       <c r="F9" s="1">
         <v>2.5</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="G9" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2.5</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1">
         <v>0</v>
@@ -1440,16 +1474,16 @@
       </c>
       <c r="AG9" s="1">
         <f>SUM(B9:AF9)</f>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>356.40259740259739</v>
+        <v>529.97938144329896</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-204.68831168831167</v>
+        <v>-378.26509572901324</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -1815,11 +1849,11 @@
       </c>
       <c r="G17" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I17" s="1">
         <f t="shared" si="2"/>
@@ -1959,7 +1993,7 @@
       <c r="AF18" s="7"/>
       <c r="AG18" s="1">
         <f>SUM(AG3:AG16)</f>
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -2320,15 +2354,15 @@
       </c>
       <c r="AH24" s="6">
         <f>SUM(AG23:AG36)</f>
-        <v>3081</v>
+        <v>3126</v>
       </c>
       <c r="AI24" s="6">
         <f>AG43</f>
-        <v>1341</v>
+        <v>1886</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>1740</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2454,7 +2488,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="1">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
@@ -2533,7 +2567,7 @@
       </c>
       <c r="AG26" s="1">
         <f t="shared" si="3"/>
-        <v>-14.285714285714286</v>
+        <v>30.714285714285715</v>
       </c>
       <c r="AH26" s="6"/>
       <c r="AI26" s="6"/>
@@ -3298,7 +3332,9 @@
       <c r="F42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G42" s="1"/>
+      <c r="G42" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -3343,7 +3379,9 @@
       <c r="F43" s="1">
         <v>26</v>
       </c>
-      <c r="G43" s="1"/>
+      <c r="G43" s="1">
+        <v>545</v>
+      </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1">
@@ -3417,7 +3455,7 @@
       </c>
       <c r="AG43" s="1">
         <f>SUM(B43:AF43)</f>
-        <v>1341</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3446,11 +3484,11 @@
       </c>
       <c r="G44" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H44" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I44" s="5">
         <f t="shared" si="5"/>
@@ -3550,7 +3588,7 @@
       </c>
       <c r="AG44" s="5">
         <f>SUM(B44:AF44)</f>
-        <v>770</v>
+        <v>970</v>
       </c>
     </row>
     <row r="45" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3580,11 +3618,11 @@
       </c>
       <c r="G46" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>645</v>
       </c>
       <c r="H46" s="5">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I46" s="5">
         <f t="shared" si="6"/>
@@ -3684,7 +3722,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>2111</v>
+        <v>2856</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Minhaz +400, vim -10
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B5156AC-BA4F-4A1F-B0C9-F020B03698E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C8CF46-7555-4B42-862A-54D6FF153DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>meal rate</t>
   </si>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -799,15 +799,15 @@
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>29.443298969072163</v>
+        <v>29.546391752577321</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>368.04123711340202</v>
+        <v>369.32989690721649</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>632.6730486008837</v>
+        <v>631.38438880706917</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -917,11 +917,11 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>338.59793814432987</v>
+        <v>339.78350515463922</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>147.11634756995585</v>
+        <v>145.93078055964651</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1031,11 +1031,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>73.608247422680407</v>
+        <v>73.86597938144331</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>-87.893961708394698</v>
+        <v>-88.151693667157602</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1143,11 +1143,11 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>515.25773195876286</v>
+        <v>517.06185567010311</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-484.54344624447714</v>
+        <v>-86.347569955817391</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1255,11 +1255,11 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>515.25773195876286</v>
+        <v>517.06185567010311</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>220.4565537555228</v>
+        <v>218.65243004418255</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1367,11 +1367,11 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>515.25773195876286</v>
+        <v>517.06185567010311</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>220.4565537555228</v>
+        <v>218.65243004418255</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1479,11 +1479,11 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>529.97938144329896</v>
+        <v>531.83505154639181</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-378.26509572901324</v>
+        <v>-380.12076583210609</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -2354,15 +2354,15 @@
       </c>
       <c r="AH24" s="6">
         <f>SUM(AG23:AG36)</f>
-        <v>3126</v>
+        <v>3526</v>
       </c>
       <c r="AI24" s="6">
         <f>AG43</f>
-        <v>1886</v>
+        <v>1896</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>1240</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2491,7 +2491,7 @@
         <v>45</v>
       </c>
       <c r="H26" s="1">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="I26" s="1">
         <v>0</v>
@@ -2567,7 +2567,7 @@
       </c>
       <c r="AG26" s="1">
         <f t="shared" si="3"/>
-        <v>30.714285714285715</v>
+        <v>430.71428571428572</v>
       </c>
       <c r="AH26" s="6"/>
       <c r="AI26" s="6"/>
@@ -3335,7 +3335,9 @@
       <c r="G42" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H42" s="1"/>
+      <c r="H42" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -3382,7 +3384,9 @@
       <c r="G43" s="1">
         <v>545</v>
       </c>
-      <c r="H43" s="1"/>
+      <c r="H43" s="1">
+        <v>10</v>
+      </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1">
         <v>0</v>
@@ -3455,7 +3459,7 @@
       </c>
       <c r="AG43" s="1">
         <f>SUM(B43:AF43)</f>
-        <v>1886</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3622,7 +3626,7 @@
       </c>
       <c r="H46" s="5">
         <f t="shared" si="6"/>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="I46" s="5">
         <f t="shared" si="6"/>
@@ -3722,7 +3726,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>2856</v>
+        <v>2866</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
moyla more -50. so total -150 for moyla
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C8CF46-7555-4B42-862A-54D6FF153DA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3552BFCB-EA5E-41F5-8BD3-735326262240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -807,7 +807,7 @@
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>631.38438880706917</v>
+        <v>624.24153166421206</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -921,7 +921,7 @@
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>145.93078055964651</v>
+        <v>138.78792341678934</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>-88.151693667157602</v>
+        <v>-95.294550810014741</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-86.347569955817391</v>
+        <v>-93.490427098674559</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>218.65243004418255</v>
+        <v>211.50957290132544</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>218.65243004418255</v>
+        <v>211.50957290132544</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-380.12076583210609</v>
+        <v>-387.26362297496325</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -2152,8 +2152,8 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1">
-        <f>-100/7</f>
-        <v>-14.285714285714286</v>
+        <f>-150/7</f>
+        <v>-21.428571428571427</v>
       </c>
       <c r="F23" s="1">
         <v>15</v>
@@ -2238,7 +2238,7 @@
       </c>
       <c r="AG23" s="1">
         <f t="shared" ref="AG23:AG36" si="3">SUM(B23:AF23)</f>
-        <v>1000.7142857142857</v>
+        <v>993.57142857142856</v>
       </c>
       <c r="AH23" s="1" t="s">
         <v>10</v>
@@ -2264,8 +2264,8 @@
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" ref="E24:E29" si="4">-100/7</f>
-        <v>-14.285714285714286</v>
+        <f t="shared" ref="E24:E29" si="4">-150/7</f>
+        <v>-21.428571428571427</v>
       </c>
       <c r="F24" s="1">
         <v>500</v>
@@ -2350,11 +2350,11 @@
       </c>
       <c r="AG24" s="1">
         <f t="shared" si="3"/>
-        <v>485.71428571428572</v>
+        <v>478.57142857142856</v>
       </c>
       <c r="AH24" s="6">
         <f>SUM(AG23:AG36)</f>
-        <v>3526</v>
+        <v>3475.9999999999995</v>
       </c>
       <c r="AI24" s="6">
         <f>AG43</f>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>1630</v>
+        <v>1579.9999999999995</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2380,7 +2380,7 @@
       </c>
       <c r="E25" s="1">
         <f t="shared" si="4"/>
-        <v>-14.285714285714286</v>
+        <v>-21.428571428571427</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1">
@@ -2463,7 +2463,7 @@
       </c>
       <c r="AG25" s="1">
         <f t="shared" si="3"/>
-        <v>-14.285714285714286</v>
+        <v>-21.428571428571427</v>
       </c>
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="E26" s="1">
         <f t="shared" si="4"/>
-        <v>-14.285714285714286</v>
+        <v>-21.428571428571427</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -2567,7 +2567,7 @@
       </c>
       <c r="AG26" s="1">
         <f t="shared" si="3"/>
-        <v>430.71428571428572</v>
+        <v>423.57142857142856</v>
       </c>
       <c r="AH26" s="6"/>
       <c r="AI26" s="6"/>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="E27" s="1">
         <f t="shared" si="4"/>
-        <v>-14.285714285714286</v>
+        <v>-21.428571428571427</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -2671,7 +2671,7 @@
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="3"/>
-        <v>735.71428571428567</v>
+        <v>728.57142857142856</v>
       </c>
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
@@ -2690,7 +2690,7 @@
       </c>
       <c r="E28" s="1">
         <f t="shared" si="4"/>
-        <v>-14.285714285714286</v>
+        <v>-21.428571428571427</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -2775,7 +2775,7 @@
       </c>
       <c r="AG28" s="1">
         <f t="shared" si="3"/>
-        <v>735.71428571428567</v>
+        <v>728.57142857142856</v>
       </c>
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="E29" s="1">
         <f t="shared" si="4"/>
-        <v>-14.285714285714286</v>
+        <v>-21.428571428571427</v>
       </c>
       <c r="F29" s="1">
         <v>-230</v>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="AG29" s="1">
         <f t="shared" si="3"/>
-        <v>151.71428571428572</v>
+        <v>144.57142857142856</v>
       </c>
       <c r="AH29" s="6"/>
       <c r="AI29" s="6"/>

</xml_diff>

<commit_message>
taher +25, forhad +25
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3552BFCB-EA5E-41F5-8BD3-735326262240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAFF540-3EF5-4FB7-A26E-A23AEDF8DE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>211.50957290132544</v>
+        <v>236.50957290132544</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>211.50957290132544</v>
+        <v>236.50957290132544</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -2354,7 +2354,7 @@
       </c>
       <c r="AH24" s="6">
         <f>SUM(AG23:AG36)</f>
-        <v>3475.9999999999995</v>
+        <v>3525.9999999999995</v>
       </c>
       <c r="AI24" s="6">
         <f>AG43</f>
@@ -2362,7 +2362,7 @@
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>1579.9999999999995</v>
+        <v>1629.9999999999995</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2595,7 +2595,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I27" s="1">
         <v>0</v>
@@ -2671,7 +2671,7 @@
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="3"/>
-        <v>728.57142857142856</v>
+        <v>753.57142857142856</v>
       </c>
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
@@ -2699,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="1">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I28" s="1">
         <v>0</v>
@@ -2775,7 +2775,7 @@
       </c>
       <c r="AG28" s="1">
         <f t="shared" si="3"/>
-        <v>728.57142857142856</v>
+        <v>753.57142857142856</v>
       </c>
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>

</xml_diff>

<commit_message>
Taher +1000, Forhad +1000
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAFF540-3EF5-4FB7-A26E-A23AEDF8DE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C6D4EF-2793-41E7-9AC5-7CA02C8E0D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,17 @@
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -508,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1270,7 @@
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>236.50957290132544</v>
+        <v>1236.5095729013253</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1371,7 +1382,7 @@
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>236.50957290132544</v>
+        <v>1236.5095729013253</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -2354,7 +2365,7 @@
       </c>
       <c r="AH24" s="6">
         <f>SUM(AG23:AG36)</f>
-        <v>3525.9999999999995</v>
+        <v>5525.9999999999991</v>
       </c>
       <c r="AI24" s="6">
         <f>AG43</f>
@@ -2362,7 +2373,7 @@
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>1629.9999999999995</v>
+        <v>3629.9999999999991</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2598,7 +2609,7 @@
         <v>25</v>
       </c>
       <c r="I27" s="1">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J27" s="1">
         <v>0</v>
@@ -2671,7 +2682,7 @@
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="3"/>
-        <v>753.57142857142856</v>
+        <v>1753.5714285714284</v>
       </c>
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
@@ -2702,7 +2713,7 @@
         <v>25</v>
       </c>
       <c r="I28" s="1">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J28" s="1">
         <v>0</v>
@@ -2775,7 +2786,7 @@
       </c>
       <c r="AG28" s="1">
         <f t="shared" si="3"/>
-        <v>753.57142857142856</v>
+        <v>1753.5714285714284</v>
       </c>
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>

</xml_diff>

<commit_message>
lobon 2 ta -40
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91377FFA-5832-4243-A03A-15B3832622CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78982FE9-1D83-4C99-B572-9C759847FD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t>meal rate</t>
   </si>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:J9"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -799,15 +799,15 @@
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>29.165217391304349</v>
+        <v>29.513043478260869</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>364.56521739130437</v>
+        <v>368.91304347826087</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>629.00621118012418</v>
+        <v>624.65838509316768</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -917,11 +917,11 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>335.40000000000003</v>
+        <v>339.4</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>143.17142857142852</v>
+        <v>139.17142857142858</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1031,11 +1031,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>72.913043478260875</v>
+        <v>73.782608695652172</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>-94.341614906832305</v>
+        <v>-95.211180124223603</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1145,11 +1145,11 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>641.63478260869567</v>
+        <v>649.28695652173906</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-218.06335403726712</v>
+        <v>-225.7155279503105</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1259,11 +1259,11 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>641.63478260869567</v>
+        <v>649.28695652173906</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>1111.9366459627327</v>
+        <v>1104.2844720496894</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1373,11 +1373,11 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>641.63478260869567</v>
+        <v>649.28695652173906</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>1111.9366459627327</v>
+        <v>1104.2844720496894</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1487,11 +1487,11 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>656.21739130434787</v>
+        <v>664.04347826086951</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-511.64596273291932</v>
+        <v>-519.47204968944095</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -2366,11 +2366,11 @@
       </c>
       <c r="AI24" s="6">
         <f>AG43</f>
-        <v>2204</v>
+        <v>2244</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>3321.9999999999991</v>
+        <v>3281.9999999999991</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3349,7 +3349,9 @@
       <c r="I42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J42" s="1"/>
+      <c r="J42" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -3401,7 +3403,7 @@
         <v>308</v>
       </c>
       <c r="J43" s="1">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="K43" s="1">
         <v>0</v>
@@ -3471,7 +3473,7 @@
       </c>
       <c r="AG43" s="1">
         <f>SUM(B43:AF43)</f>
-        <v>2204</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3646,7 +3648,7 @@
       </c>
       <c r="J46" s="5">
         <f t="shared" si="6"/>
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="K46" s="5">
         <f t="shared" si="6"/>
@@ -3738,7 +3740,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>3354</v>
+        <v>3394</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Himel guest, Moricher gura -10
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0747467-06E2-4469-A344-2BF13947DD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CD2A3F-7BC2-4F5D-92F7-FF20FC6DC9A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:K9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -799,15 +799,15 @@
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>29.846743295019156</v>
+        <v>29.548872180451127</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>373.08429118773944</v>
+        <v>369.36090225563908</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>620.48713738368906</v>
+        <v>624.21052631578948</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -917,11 +917,11 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>343.23754789272027</v>
+        <v>339.81203007518798</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>135.33388067870828</v>
+        <v>138.75939849624058</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -959,7 +959,7 @@
         <v>3</v>
       </c>
       <c r="K5" s="1">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="L5" s="1">
         <v>0</v>
@@ -1026,16 +1026,16 @@
       </c>
       <c r="AG5" s="1">
         <f t="shared" ref="AG5:AG16" si="1">SUM(B5:AF5)</f>
-        <v>8</v>
+        <v>10.5</v>
       </c>
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>238.77394636015325</v>
+        <v>310.26315789473682</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>-260.20251778872466</v>
+        <v>-331.69172932330827</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1145,11 +1145,11 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>731.24521072796927</v>
+        <v>723.9473684210526</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-307.67378215654071</v>
+        <v>-300.37593984962405</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1259,11 +1259,11 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>731.24521072796927</v>
+        <v>723.9473684210526</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>1022.3262178434592</v>
+        <v>1029.624060150376</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1373,11 +1373,11 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>731.24521072796927</v>
+        <v>723.9473684210526</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>1022.3262178434592</v>
+        <v>1029.624060150376</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1487,11 +1487,11 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>746.16858237547888</v>
+        <v>738.72180451127815</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-601.59715380405032</v>
+        <v>-594.1503759398496</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -1873,7 +1873,7 @@
       </c>
       <c r="K17" s="1">
         <f t="shared" si="2"/>
-        <v>12.5</v>
+        <v>15</v>
       </c>
       <c r="L17" s="1">
         <f t="shared" si="2"/>
@@ -2001,7 +2001,7 @@
       <c r="AF18" s="7"/>
       <c r="AG18" s="1">
         <f>SUM(AG3:AG16)</f>
-        <v>130.5</v>
+        <v>133</v>
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -2366,11 +2366,11 @@
       </c>
       <c r="AI24" s="6">
         <f>AG43</f>
-        <v>2590</v>
+        <v>2600</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>2935.9999999999991</v>
+        <v>2925.9999999999991</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3406,7 +3406,7 @@
         <v>386</v>
       </c>
       <c r="K43" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L43" s="1">
         <v>0</v>
@@ -3473,7 +3473,7 @@
       </c>
       <c r="AG43" s="1">
         <f>SUM(B43:AF43)</f>
-        <v>2590</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3518,7 +3518,7 @@
       </c>
       <c r="K44" s="5">
         <f t="shared" si="5"/>
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="L44" s="5">
         <f t="shared" si="5"/>
@@ -3606,7 +3606,7 @@
       </c>
       <c r="AG44" s="5">
         <f>SUM(B44:AF44)</f>
-        <v>1305</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="45" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3652,7 +3652,7 @@
       </c>
       <c r="K46" s="5">
         <f t="shared" si="6"/>
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="L46" s="5">
         <f t="shared" si="6"/>
@@ -3740,7 +3740,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>3895</v>
+        <v>3930</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Rakib & Mahfuz meal on from Noon, 12th March
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B1C78D-97E5-447D-B327-5A3ABE98530A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94CCD59-43C0-4CAF-B2CA-90AE794C0735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,7 +508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F18" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -734,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N3" s="1">
         <v>0</v>
@@ -795,19 +795,19 @@
       </c>
       <c r="AG3" s="1">
         <f>SUM(B3:AF3)</f>
-        <v>12.5</v>
+        <v>14.5</v>
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>30.490566037735849</v>
+        <v>29.987730061349694</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>381.1320754716981</v>
+        <v>434.82208588957059</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>612.4393530997304</v>
+        <v>558.74934268185802</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
       <c r="M4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N4" s="1">
         <v>0</v>
@@ -912,16 +912,16 @@
       </c>
       <c r="AG4" s="1">
         <f>SUM(B4:AF4)</f>
-        <v>11.5</v>
+        <v>13.5</v>
       </c>
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>350.64150943396226</v>
+        <v>404.83435582822085</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>127.9299191374663</v>
+        <v>73.737072743207705</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1031,11 +1031,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>503.09433962264154</v>
+        <v>494.79754601226995</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>1475.4770889487872</v>
+        <v>1483.7738825591587</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1145,11 +1145,11 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>899.47169811320759</v>
+        <v>884.63803680981596</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-475.90026954177904</v>
+        <v>-461.0666082383874</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1259,11 +1259,11 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>899.47169811320759</v>
+        <v>884.63803680981596</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>854.09973045822085</v>
+        <v>868.93339176161248</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1373,11 +1373,11 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>899.47169811320759</v>
+        <v>884.63803680981596</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>854.09973045822085</v>
+        <v>868.93339176161248</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1487,11 +1487,11 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>914.71698113207549</v>
+        <v>899.63190184049085</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-770.14555256064693</v>
+        <v>-755.0604732690623</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="M17" s="1">
         <f t="shared" si="2"/>
-        <v>13.5</v>
+        <v>17.5</v>
       </c>
       <c r="N17" s="1">
         <f t="shared" si="2"/>
@@ -2001,7 +2001,7 @@
       <c r="AF18" s="7"/>
       <c r="AG18" s="1">
         <f>SUM(AG3:AG16)</f>
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -3528,7 +3528,7 @@
       </c>
       <c r="M44" s="5">
         <f t="shared" si="5"/>
-        <v>135</v>
+        <v>175</v>
       </c>
       <c r="N44" s="5">
         <f t="shared" si="5"/>
@@ -3608,7 +3608,7 @@
       </c>
       <c r="AG44" s="5">
         <f>SUM(B44:AF44)</f>
-        <v>1590</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="45" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3662,7 +3662,7 @@
       </c>
       <c r="M46" s="5">
         <f t="shared" si="6"/>
-        <v>135</v>
+        <v>175</v>
       </c>
       <c r="N46" s="5">
         <f t="shared" si="6"/>
@@ -3742,7 +3742,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>4848</v>
+        <v>4888</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added rice cost to cost formula =SUM(AG43+AG44)
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954E611D-C651-442B-ACF4-6C51457E000D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C951E2D5-B579-49FF-8027-FA64E52B01CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AI24" sqref="AI24:AI29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2365,12 +2365,12 @@
         <v>7526</v>
       </c>
       <c r="AI24" s="6">
-        <f>AG43</f>
-        <v>3258</v>
+        <f>SUM(AG43+AG44)</f>
+        <v>4528</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>4268</v>
+        <v>2998</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3546,43 +3546,33 @@
         <v>0</v>
       </c>
       <c r="W44" s="5">
-        <f t="shared" ref="C44:AF44" si="5">W17*0.2*50</f>
         <v>0</v>
       </c>
       <c r="X44" s="5">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y44" s="5">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z44" s="5">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA44" s="5">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB44" s="5">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC44" s="5">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AD44" s="5">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE44" s="5">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AF44" s="5">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AG44" s="5">
@@ -3600,123 +3590,123 @@
         <v>1655</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" ref="C46:AF46" si="6">SUM(C43+C44)</f>
+        <f t="shared" ref="C46:AF46" si="5">SUM(C43+C44)</f>
         <v>415</v>
       </c>
       <c r="D46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>515</v>
       </c>
       <c r="F46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
       <c r="G46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>545</v>
       </c>
       <c r="H46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="I46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>308</v>
       </c>
       <c r="J46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>386</v>
       </c>
       <c r="K46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="L46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>658</v>
       </c>
       <c r="M46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="N46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="V46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="W46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="X46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Y46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Z46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AA46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AB46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AD46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AE46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AF46" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AG46" s="5">

</xml_diff>

<commit_message>
rice 1.4 kg -77
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C951E2D5-B579-49FF-8027-FA64E52B01CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCACB84A-6803-419D-A794-7B702AAF528B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI24" sqref="AI24:AI29"/>
+    <sheetView tabSelected="1" topLeftCell="J18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -799,15 +799,15 @@
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>27.779141104294478</v>
+        <v>28.25153374233129</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>402.79754601226995</v>
+        <v>409.64723926380373</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>590.77388255915866</v>
+        <v>583.92418930762483</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -917,11 +917,11 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>375.01840490797548</v>
+        <v>381.39570552147239</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>103.55302366345308</v>
+        <v>97.175723049956162</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1031,11 +1031,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>458.35582822085888</v>
+        <v>466.15030674846628</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>1520.2156003505697</v>
+        <v>1512.4211218229625</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1145,11 +1145,11 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>819.48466257668713</v>
+        <v>833.42024539877309</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-395.91323400525857</v>
+        <v>-409.84881682734454</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1259,11 +1259,11 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>819.48466257668713</v>
+        <v>833.42024539877309</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>934.08676599474131</v>
+        <v>920.15118317265535</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1373,11 +1373,11 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>819.48466257668713</v>
+        <v>833.42024539877309</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>934.08676599474131</v>
+        <v>920.15118317265535</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1487,11 +1487,11 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>833.37423312883436</v>
+        <v>847.54601226993873</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-688.80280455740581</v>
+        <v>-702.97458369851017</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -2366,11 +2366,11 @@
       </c>
       <c r="AI24" s="6">
         <f>SUM(AG43+AG44)</f>
-        <v>4528</v>
+        <v>4605</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>2998</v>
+        <v>2921</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3516,7 +3516,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="5">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="N44" s="5">
         <v>0</v>
@@ -3577,7 +3577,7 @@
       </c>
       <c r="AG44" s="5">
         <f>SUM(B44:AF44)</f>
-        <v>1270</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="45" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3631,7 +3631,7 @@
       </c>
       <c r="M46" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="N46" s="5">
         <f t="shared" si="5"/>
@@ -3711,7 +3711,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>4528</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Taher+250, Forhad+250, Himel-10, Bazar -750
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCACB84A-6803-419D-A794-7B702AAF528B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F221F282-B471-4FB1-9F68-14C8DBAC4CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>meal rate</t>
   </si>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+    <sheetView tabSelected="1" topLeftCell="I13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -799,15 +799,15 @@
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>28.25153374233129</v>
+        <v>48.190184049079754</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>409.64723926380373</v>
+        <v>698.75766871165638</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>583.92418930762483</v>
+        <v>294.81375985977218</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -917,11 +917,11 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>381.39570552147239</v>
+        <v>650.5674846625767</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>97.175723049956162</v>
+        <v>-171.99605609114815</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1031,11 +1031,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>466.15030674846628</v>
+        <v>795.13803680981596</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>1512.4211218229625</v>
+        <v>1173.4333917616127</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1145,11 +1145,11 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>833.42024539877309</v>
+        <v>1421.6104294478528</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-409.84881682734454</v>
+        <v>-998.03900087642421</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1259,11 +1259,11 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>833.42024539877309</v>
+        <v>1421.6104294478528</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>920.15118317265535</v>
+        <v>581.96099912357568</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1373,11 +1373,11 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>833.42024539877309</v>
+        <v>1421.6104294478528</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>920.15118317265535</v>
+        <v>581.96099912357568</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1487,11 +1487,11 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>847.54601226993873</v>
+        <v>1445.7055214723925</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-702.97458369851017</v>
+        <v>-1301.1340929009639</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -2362,15 +2362,15 @@
       </c>
       <c r="AH24" s="6">
         <f>SUM(AG23:AG36)</f>
-        <v>7526</v>
+        <v>8016</v>
       </c>
       <c r="AI24" s="6">
         <f>SUM(AG43+AG44)</f>
-        <v>4605</v>
+        <v>7855</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>2921</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2413,7 +2413,7 @@
         <v>0</v>
       </c>
       <c r="N25" s="1">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="O25" s="1">
         <v>0</v>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AG25" s="1">
         <f t="shared" si="3"/>
-        <v>1978.5714285714287</v>
+        <v>1968.5714285714287</v>
       </c>
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
@@ -2621,7 +2621,7 @@
         <v>0</v>
       </c>
       <c r="N27" s="1">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="O27" s="1">
         <v>0</v>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="3"/>
-        <v>1753.5714285714284</v>
+        <v>2003.5714285714284</v>
       </c>
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
@@ -2725,7 +2725,7 @@
         <v>0</v>
       </c>
       <c r="N28" s="1">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="O28" s="1">
         <v>0</v>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="AG28" s="1">
         <f t="shared" si="3"/>
-        <v>1753.5714285714284</v>
+        <v>2003.5714285714284</v>
       </c>
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>
@@ -3357,7 +3357,9 @@
         <v>16</v>
       </c>
       <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
+      <c r="N42" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
@@ -3417,7 +3419,7 @@
         <v>0</v>
       </c>
       <c r="N43" s="1">
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="O43" s="1">
         <v>0</v>
@@ -3475,7 +3477,7 @@
       </c>
       <c r="AG43" s="1">
         <f>SUM(B43:AF43)</f>
-        <v>3258</v>
+        <v>4008</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3519,7 +3521,7 @@
         <v>77</v>
       </c>
       <c r="N44" s="5">
-        <v>0</v>
+        <v>2500</v>
       </c>
       <c r="O44" s="5">
         <v>0</v>
@@ -3577,7 +3579,7 @@
       </c>
       <c r="AG44" s="5">
         <f>SUM(B44:AF44)</f>
-        <v>1347</v>
+        <v>3847</v>
       </c>
     </row>
     <row r="45" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3635,7 +3637,7 @@
       </c>
       <c r="N46" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3250</v>
       </c>
       <c r="O46" s="5">
         <f t="shared" si="5"/>
@@ -3711,7 +3713,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>4605</v>
+        <v>7855</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
shokal off, rakib&himel night off
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3047B83-F7DF-434E-AE0E-50A0B75959C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3288486-34A0-48F1-B9CA-CCE344179D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="A1:AK1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -740,7 +740,7 @@
         <v>2.5</v>
       </c>
       <c r="O3" s="1">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="P3" s="1">
         <v>0</v>
@@ -795,19 +795,19 @@
       </c>
       <c r="AG3" s="1">
         <f>SUM(B3:AF3)</f>
-        <v>19.5</v>
+        <v>18</v>
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>40.489690721649481</v>
+        <v>41.671087533156502</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>789.54896907216494</v>
+        <v>750.07957559681699</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>204.02245949926362</v>
+        <v>243.49185297461156</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -857,7 +857,7 @@
         <v>2.5</v>
       </c>
       <c r="O4" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="P4" s="1">
         <v>0</v>
@@ -912,16 +912,16 @@
       </c>
       <c r="AG4" s="1">
         <f>SUM(B4:AF4)</f>
-        <v>18.5</v>
+        <v>18</v>
       </c>
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>749.05927835051534</v>
+        <v>750.07957559681699</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>-270.48784977908679</v>
+        <v>-271.50814702538844</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -971,7 +971,7 @@
         <v>1.5</v>
       </c>
       <c r="O5" s="1">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="P5" s="1">
         <v>0</v>
@@ -1026,16 +1026,16 @@
       </c>
       <c r="AG5" s="1">
         <f t="shared" ref="AG5:AG16" si="1">SUM(B5:AF5)</f>
-        <v>20.5</v>
+        <v>19</v>
       </c>
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>830.0386597938143</v>
+        <v>791.75066312997353</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>1138.5327687776144</v>
+        <v>1176.820765441455</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1085,7 +1085,7 @@
         <v>1.5</v>
       </c>
       <c r="O6" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="P6" s="1">
         <v>0</v>
@@ -1140,16 +1140,16 @@
       </c>
       <c r="AG6" s="1">
         <f t="shared" si="1"/>
-        <v>33.5</v>
+        <v>33</v>
       </c>
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>1356.4046391752577</v>
+        <v>1375.1458885941645</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-932.83321060382912</v>
+        <v>-951.57446002273593</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1199,7 +1199,7 @@
         <v>0.5</v>
       </c>
       <c r="O7" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
@@ -1254,16 +1254,16 @@
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="1"/>
-        <v>32.5</v>
+        <v>32</v>
       </c>
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>1315.9149484536081</v>
+        <v>1333.4748010610081</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>687.65648011782037</v>
+        <v>670.09662751042038</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1313,7 +1313,7 @@
         <v>2.5</v>
       </c>
       <c r="O8" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="P8" s="1">
         <v>0</v>
@@ -1368,16 +1368,16 @@
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="1"/>
-        <v>34.5</v>
+        <v>34</v>
       </c>
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>1396.894329896907</v>
+        <v>1416.8169761273211</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>606.6770986745214</v>
+        <v>586.7544524441073</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1427,7 +1427,7 @@
         <v>2.5</v>
       </c>
       <c r="O9" s="1">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="P9" s="1">
         <v>0</v>
@@ -1482,16 +1482,16 @@
       </c>
       <c r="AG9" s="1">
         <f>SUM(B9:AF9)</f>
-        <v>35</v>
+        <v>34.5</v>
       </c>
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>1417.1391752577319</v>
+        <v>1437.6525198938994</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-1272.5677466863035</v>
+        <v>-1293.0810913224709</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -1889,7 +1889,7 @@
       </c>
       <c r="O17" s="1">
         <f t="shared" si="2"/>
-        <v>17.5</v>
+        <v>12</v>
       </c>
       <c r="P17" s="1">
         <f t="shared" si="2"/>
@@ -2001,7 +2001,7 @@
       <c r="AF18" s="7"/>
       <c r="AG18" s="1">
         <f>SUM(AG3:AG16)</f>
-        <v>194</v>
+        <v>188.5</v>
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>

</xml_diff>

<commit_message>
Bazar -213(oil300,lau,begun,alu,piyaj,motaDal,chotoDal), Taher+250, Forhad+250, Himel+200
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3288486-34A0-48F1-B9CA-CCE344179D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4EA1EB-8C14-40EF-964E-710017C19525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>meal rate</t>
   </si>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="F17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -799,15 +799,15 @@
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>41.671087533156502</v>
+        <v>42.801061007957557</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>750.07957559681699</v>
+        <v>770.41909814323606</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>243.49185297461156</v>
+        <v>223.1523304281925</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -917,11 +917,11 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>750.07957559681699</v>
+        <v>770.41909814323606</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>-271.50814702538844</v>
+        <v>-291.8476695718075</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1031,11 +1031,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>791.75066312997353</v>
+        <v>813.22015915119357</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>1176.820765441455</v>
+        <v>1355.351269420235</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1145,11 +1145,11 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>1375.1458885941645</v>
+        <v>1412.4350132625993</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-951.57446002273593</v>
+        <v>-988.86358469117079</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1259,11 +1259,11 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>1333.4748010610081</v>
+        <v>1369.6339522546418</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>670.09662751042038</v>
+        <v>883.93747631678661</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1373,11 +1373,11 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>1416.8169761273211</v>
+        <v>1455.2360742705569</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>586.7544524441073</v>
+        <v>798.33535430087159</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1487,11 +1487,11 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>1437.6525198938994</v>
+        <v>1476.6366047745357</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-1293.0810913224709</v>
+        <v>-1332.0651762031071</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -2362,15 +2362,15 @@
       </c>
       <c r="AH24" s="6">
         <f>SUM(AG23:AG36)</f>
-        <v>8016</v>
+        <v>8716</v>
       </c>
       <c r="AI24" s="6">
         <f>SUM(AG43+AG44)</f>
-        <v>7855</v>
+        <v>8068</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>161</v>
+        <v>648</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2416,7 +2416,7 @@
         <v>-10</v>
       </c>
       <c r="O25" s="1">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="P25" s="1">
         <v>0</v>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AG25" s="1">
         <f t="shared" si="3"/>
-        <v>1968.5714285714287</v>
+        <v>2168.5714285714284</v>
       </c>
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
@@ -2624,7 +2624,7 @@
         <v>250</v>
       </c>
       <c r="O27" s="1">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="P27" s="1">
         <v>0</v>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="3"/>
-        <v>2003.5714285714284</v>
+        <v>2253.5714285714284</v>
       </c>
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
@@ -2728,7 +2728,7 @@
         <v>250</v>
       </c>
       <c r="O28" s="1">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="P28" s="1">
         <v>0</v>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="AG28" s="1">
         <f t="shared" si="3"/>
-        <v>2003.5714285714284</v>
+        <v>2253.5714285714284</v>
       </c>
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>
@@ -3360,7 +3360,9 @@
       <c r="N42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O42" s="1"/>
+      <c r="O42" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
@@ -3422,7 +3424,7 @@
         <v>750</v>
       </c>
       <c r="O43" s="1">
-        <v>0</v>
+        <v>213</v>
       </c>
       <c r="P43" s="1">
         <v>0</v>
@@ -3477,7 +3479,7 @@
       </c>
       <c r="AG43" s="1">
         <f>SUM(B43:AF43)</f>
-        <v>4008</v>
+        <v>4221</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3641,7 +3643,7 @@
       </c>
       <c r="O46" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>213</v>
       </c>
       <c r="P46" s="5">
         <f t="shared" si="5"/>
@@ -3713,7 +3715,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>7855</v>
+        <v>8068</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Himel bazar-851,vim-10,Himel raat off,dupur extra+2meal
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2913D82-63DB-4E2E-8809-ADE8F565EBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C767D3-5405-4892-A551-C1B1242A5DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>meal rate</t>
   </si>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -752,10 +752,10 @@
         <v>2.5</v>
       </c>
       <c r="S3" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="T3" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="U3" s="1">
         <v>0</v>
@@ -795,19 +795,19 @@
       </c>
       <c r="AG3" s="1">
         <f>SUM(B3:AF3)</f>
-        <v>25.5</v>
+        <v>30.5</v>
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>36.879668049792528</v>
+        <v>35.194945848375454</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>940.43153526970946</v>
+        <v>1073.4458483754513</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>53.139893301719098</v>
+        <v>-79.87441980402275</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -869,10 +869,10 @@
         <v>2.5</v>
       </c>
       <c r="S4" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="T4" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="U4" s="1">
         <v>0</v>
@@ -912,16 +912,16 @@
       </c>
       <c r="AG4" s="1">
         <f>SUM(B4:AF4)</f>
-        <v>25.5</v>
+        <v>30.5</v>
       </c>
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>940.43153526970946</v>
+        <v>1073.4458483754513</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>538.13989330171898</v>
+        <v>405.12558019597714</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -983,10 +983,10 @@
         <v>2.5</v>
       </c>
       <c r="S5" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="T5" s="1">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="U5" s="1">
         <v>0</v>
@@ -1026,16 +1026,16 @@
       </c>
       <c r="AG5" s="1">
         <f t="shared" ref="AG5:AG16" si="1">SUM(B5:AF5)</f>
-        <v>26.5</v>
+        <v>32.5</v>
       </c>
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>977.31120331950194</v>
+        <v>1143.8357400722023</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>1191.2602252519264</v>
+        <v>1029.7356884992262</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1097,10 +1097,10 @@
         <v>2.5</v>
       </c>
       <c r="S6" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="T6" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="U6" s="1">
         <v>0</v>
@@ -1140,16 +1140,16 @@
       </c>
       <c r="AG6" s="1">
         <f t="shared" si="1"/>
-        <v>40.5</v>
+        <v>45.5</v>
       </c>
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>1493.6265560165973</v>
+        <v>1601.3700361010831</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-170.05512744516886</v>
+        <v>-277.79860752965465</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1211,10 +1211,10 @@
         <v>2.5</v>
       </c>
       <c r="S7" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="T7" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="U7" s="1">
         <v>0</v>
@@ -1254,16 +1254,16 @@
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="1"/>
-        <v>39.5</v>
+        <v>44.5</v>
       </c>
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>1456.7468879668049</v>
+        <v>1566.1750902527076</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>796.82454060462351</v>
+        <v>687.39633831872084</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1325,10 +1325,10 @@
         <v>2.5</v>
       </c>
       <c r="S8" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="T8" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="U8" s="1">
         <v>0</v>
@@ -1368,16 +1368,16 @@
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="1"/>
-        <v>41.5</v>
+        <v>46.5</v>
       </c>
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>1530.5062240663899</v>
+        <v>1636.5649819494586</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>723.06520450503854</v>
+        <v>617.00644662196987</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1439,10 +1439,10 @@
         <v>2.5</v>
       </c>
       <c r="S9" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="T9" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="U9" s="1">
         <v>0</v>
@@ -1482,16 +1482,16 @@
       </c>
       <c r="AG9" s="1">
         <f>SUM(B9:AF9)</f>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>1548.9460580912862</v>
+        <v>1654.1624548736463</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-1404.3746295198575</v>
+        <v>-1509.5910263022179</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -1905,11 +1905,11 @@
       </c>
       <c r="S17" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="T17" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="U17" s="1">
         <f t="shared" si="2"/>
@@ -2001,7 +2001,7 @@
       <c r="AF18" s="7"/>
       <c r="AG18" s="1">
         <f>SUM(AG3:AG16)</f>
-        <v>241</v>
+        <v>277</v>
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -2362,15 +2362,15 @@
       </c>
       <c r="AH24" s="6">
         <f>SUM(AG23:AG36)</f>
-        <v>10615.999999999998</v>
+        <v>10620.999999999998</v>
       </c>
       <c r="AI24" s="6">
         <f>SUM(AG43+AG44)</f>
-        <v>8888</v>
+        <v>9749</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>1727.9999999999982</v>
+        <v>871.99999999999818</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
         <v>0</v>
       </c>
       <c r="S25" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T25" s="1">
         <v>0</v>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AG25" s="1">
         <f t="shared" si="3"/>
-        <v>2168.5714285714284</v>
+        <v>2173.5714285714284</v>
       </c>
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
@@ -3368,7 +3368,9 @@
         <v>5</v>
       </c>
       <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
+      <c r="S42" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
@@ -3438,10 +3440,10 @@
         <v>20</v>
       </c>
       <c r="S43" s="1">
-        <v>0</v>
+        <v>851</v>
       </c>
       <c r="T43" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U43" s="1">
         <v>0</v>
@@ -3481,7 +3483,7 @@
       </c>
       <c r="AG43" s="1">
         <f>SUM(B43:AF43)</f>
-        <v>5041</v>
+        <v>5902</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3661,11 +3663,11 @@
       </c>
       <c r="S46" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>851</v>
       </c>
       <c r="T46" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U46" s="5">
         <f t="shared" si="5"/>
@@ -3717,7 +3719,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>8888</v>
+        <v>9749</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
dal + roshun = 24
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C767D3-5405-4892-A551-C1B1242A5DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751CD466-4C41-4D1D-9893-F67ED6A8E089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="A1:AK1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="T44" sqref="T44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -799,15 +799,15 @@
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>35.194945848375454</v>
+        <v>35.281588447653426</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>1073.4458483754513</v>
+        <v>1076.0884476534295</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>-79.87441980402275</v>
+        <v>-82.517019082000957</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -917,11 +917,11 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>1073.4458483754513</v>
+        <v>1076.0884476534295</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>405.12558019597714</v>
+        <v>402.48298091799893</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1031,11 +1031,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>1143.8357400722023</v>
+        <v>1146.6516245487364</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>1029.7356884992262</v>
+        <v>1026.919804022692</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1145,11 +1145,11 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>1601.3700361010831</v>
+        <v>1605.3122743682309</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-277.79860752965465</v>
+        <v>-281.74084579680243</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1259,11 +1259,11 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>1566.1750902527076</v>
+        <v>1570.0306859205775</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>687.39633831872084</v>
+        <v>683.54074265085092</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1373,11 +1373,11 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>1636.5649819494586</v>
+        <v>1640.5938628158842</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>617.00644662196987</v>
+        <v>612.97756575554422</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1487,11 +1487,11 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>1654.1624548736463</v>
+        <v>1658.234657039711</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-1509.5910263022179</v>
+        <v>-1513.6632284682823</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -2366,11 +2366,11 @@
       </c>
       <c r="AI24" s="6">
         <f>SUM(AG43+AG44)</f>
-        <v>9749</v>
+        <v>9773</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>871.99999999999818</v>
+        <v>847.99999999999818</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3443,7 +3443,7 @@
         <v>851</v>
       </c>
       <c r="T43" s="1">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="U43" s="1">
         <v>0</v>
@@ -3483,7 +3483,7 @@
       </c>
       <c r="AG43" s="1">
         <f>SUM(B43:AF43)</f>
-        <v>5902</v>
+        <v>5926</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3667,7 +3667,7 @@
       </c>
       <c r="T46" s="5">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="U46" s="5">
         <f t="shared" si="5"/>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>9749</v>
+        <v>9773</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Rakib&Mahfuz 19 tarikh meal= 1.5 each jelaSomity
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B9D51A-EF3D-4B4E-81C3-80C551A288AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D417963-8CC2-402E-9E01-3D05CB591712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3:V9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -755,7 +755,7 @@
         <v>2.5</v>
       </c>
       <c r="T3" s="1">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="U3" s="1">
         <v>2.5</v>
@@ -795,19 +795,19 @@
       </c>
       <c r="AG3" s="1">
         <f>SUM(B3:AF3)</f>
-        <v>35.5</v>
+        <v>34.5</v>
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>33.08653846153846</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>1174.5721153846152</v>
+        <v>1148.8499999999999</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>-181.00068681318669</v>
+        <v>-155.27857142857135</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -872,7 +872,7 @@
         <v>2.5</v>
       </c>
       <c r="T4" s="1">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="U4" s="1">
         <v>2.5</v>
@@ -912,16 +912,16 @@
       </c>
       <c r="AG4" s="1">
         <f>SUM(B4:AF4)</f>
-        <v>35.5</v>
+        <v>34.5</v>
       </c>
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>1174.5721153846152</v>
+        <v>1148.8499999999999</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>303.9993131868132</v>
+        <v>329.72142857142853</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1031,11 +1031,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>1240.7451923076922</v>
+        <v>1248.75</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>932.82623626373629</v>
+        <v>924.82142857142844</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1145,11 +1145,11 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>1670.8701923076922</v>
+        <v>1681.6499999999999</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-347.29876373626371</v>
+        <v>-358.07857142857142</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1259,11 +1259,11 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>1637.7836538461538</v>
+        <v>1648.35</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>615.78777472527463</v>
+        <v>605.22142857142853</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1373,11 +1373,11 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>1703.9567307692307</v>
+        <v>1714.9499999999998</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>549.61469780219772</v>
+        <v>538.62142857142862</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1487,11 +1487,11 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>1720.5</v>
+        <v>1731.6</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-1575.9285714285716</v>
+        <v>-1587.0285714285715</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -1909,7 +1909,7 @@
       </c>
       <c r="T17" s="1">
         <f t="shared" si="2"/>
-        <v>18.5</v>
+        <v>16.5</v>
       </c>
       <c r="U17" s="1">
         <f t="shared" si="2"/>
@@ -2001,7 +2001,7 @@
       <c r="AF18" s="7"/>
       <c r="AG18" s="1">
         <f>SUM(AG3:AG16)</f>
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>

</xml_diff>

<commit_message>
tel 500g -98, Minhaz raat vat short. meal -1
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BF51B0-0C42-49FF-B561-BE19C468CA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FD687A-CC96-4782-A303-C5A2976BFCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>meal rate</t>
   </si>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -799,15 +799,15 @@
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>33.299999999999997</v>
+        <v>33.724919093851135</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>1148.8499999999999</v>
+        <v>1163.5097087378642</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>-155.27857142857135</v>
+        <v>-169.93828016643567</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -917,11 +917,11 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>1148.8499999999999</v>
+        <v>1163.5097087378642</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>329.72142857142853</v>
+        <v>315.06171983356421</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1031,11 +1031,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>1248.75</v>
+        <v>1264.6844660194176</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>924.82142857142844</v>
+        <v>908.8869625520108</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1106,7 +1106,7 @@
         <v>2.5</v>
       </c>
       <c r="V6" s="1">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="W6" s="1">
         <v>0</v>
@@ -1140,16 +1140,16 @@
       </c>
       <c r="AG6" s="1">
         <f t="shared" si="1"/>
-        <v>50.5</v>
+        <v>49.5</v>
       </c>
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>1681.6499999999999</v>
+        <v>1669.3834951456311</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-358.07857142857142</v>
+        <v>-345.81206657420262</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1259,11 +1259,11 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>1648.35</v>
+        <v>1669.3834951456311</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>605.22142857142853</v>
+        <v>584.18793342579738</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1373,11 +1373,11 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>1714.9499999999998</v>
+        <v>1736.8333333333335</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>538.62142857142862</v>
+        <v>516.73809523809496</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1487,11 +1487,11 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>1731.6</v>
+        <v>1753.695792880259</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-87.028571428571468</v>
+        <v>-109.12436430883054</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="V17" s="1">
         <f t="shared" si="2"/>
-        <v>17.5</v>
+        <v>16.5</v>
       </c>
       <c r="W17" s="1">
         <f t="shared" si="2"/>
@@ -2001,7 +2001,7 @@
       <c r="AF18" s="7"/>
       <c r="AG18" s="1">
         <f>SUM(AG3:AG16)</f>
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -2366,11 +2366,11 @@
       </c>
       <c r="AI24" s="6">
         <f>SUM(AG43+AG44)</f>
-        <v>10323</v>
+        <v>10421</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>1797.9999999999964</v>
+        <v>1699.9999999999964</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3375,7 +3375,9 @@
       <c r="U42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V42" s="1"/>
+      <c r="V42" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
@@ -3451,7 +3453,7 @@
         <v>550</v>
       </c>
       <c r="V43" s="1">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="W43" s="1">
         <v>0</v>
@@ -3485,7 +3487,7 @@
       </c>
       <c r="AG43" s="1">
         <f>SUM(B43:AF43)</f>
-        <v>6476</v>
+        <v>6574</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3677,7 +3679,7 @@
       </c>
       <c r="V46" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="W46" s="5">
         <f t="shared" si="5"/>
@@ -3721,7 +3723,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>10323</v>
+        <v>10421</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
bazar-840, Himel-430, shil_pata-70(-10 each)
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FD687A-CC96-4782-A303-C5A2976BFCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF2ED56-159D-49F1-B526-548965C611D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
     <t>meal rate</t>
   </si>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView tabSelected="1" topLeftCell="H18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W44" sqref="W44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -799,15 +799,15 @@
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>33.724919093851135</v>
+        <v>36.443365695792878</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>1163.5097087378642</v>
+        <v>1257.2961165048544</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>-169.93828016643567</v>
+        <v>-273.7246879334258</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -917,11 +917,11 @@
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>1163.5097087378642</v>
+        <v>1257.2961165048544</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>315.06171983356421</v>
+        <v>211.27531206657409</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -1031,11 +1031,11 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>1264.6844660194176</v>
+        <v>1366.6262135922329</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>908.8869625520108</v>
+        <v>366.9452149791955</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1145,11 +1145,11 @@
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>1669.3834951456311</v>
+        <v>1803.9466019417475</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-345.81206657420262</v>
+        <v>-490.37517337031909</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1259,11 +1259,11 @@
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>1669.3834951456311</v>
+        <v>1803.9466019417475</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>584.18793342579738</v>
+        <v>439.62482662968091</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1373,11 +1373,11 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>1736.8333333333335</v>
+        <v>1876.8333333333333</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>516.73809523809496</v>
+        <v>366.73809523809518</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1487,11 +1487,11 @@
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>1753.695792880259</v>
+        <v>1895.0550161812296</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-109.12436430883054</v>
+        <v>-260.48358760980113</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -2215,7 +2215,7 @@
         <v>0</v>
       </c>
       <c r="W23" s="1">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="X23" s="1">
         <v>0</v>
@@ -2246,7 +2246,7 @@
       </c>
       <c r="AG23" s="1">
         <f t="shared" ref="AG23:AG36" si="3">SUM(B23:AF23)</f>
-        <v>993.57142857142856</v>
+        <v>983.57142857142856</v>
       </c>
       <c r="AH23" s="1" t="s">
         <v>10</v>
@@ -2327,7 +2327,7 @@
         <v>0</v>
       </c>
       <c r="W24" s="1">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="X24" s="1">
         <v>0</v>
@@ -2358,19 +2358,19 @@
       </c>
       <c r="AG24" s="1">
         <f t="shared" si="3"/>
-        <v>1478.5714285714284</v>
+        <v>1468.5714285714284</v>
       </c>
       <c r="AH24" s="6">
         <f>SUM(AG23:AG36)</f>
-        <v>12120.999999999996</v>
+        <v>11621</v>
       </c>
       <c r="AI24" s="6">
         <f>SUM(AG43+AG44)</f>
-        <v>10421</v>
+        <v>11261</v>
       </c>
       <c r="AJ24" s="6">
         <f>AH24-AI24</f>
-        <v>1699.9999999999964</v>
+        <v>360</v>
       </c>
     </row>
     <row r="25" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2437,10 +2437,10 @@
         <v>0</v>
       </c>
       <c r="V25" s="1">
-        <v>0</v>
+        <v>-430</v>
       </c>
       <c r="W25" s="1">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="X25" s="1">
         <v>0</v>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="AG25" s="1">
         <f t="shared" si="3"/>
-        <v>2173.5714285714284</v>
+        <v>1733.5714285714284</v>
       </c>
       <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
@@ -2544,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="W26" s="1">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="X26" s="1">
         <v>0</v>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="AG26" s="1">
         <f t="shared" si="3"/>
-        <v>1323.5714285714284</v>
+        <v>1313.5714285714284</v>
       </c>
       <c r="AH26" s="6"/>
       <c r="AI26" s="6"/>
@@ -2648,7 +2648,7 @@
         <v>0</v>
       </c>
       <c r="W27" s="1">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="X27" s="1">
         <v>0</v>
@@ -2679,7 +2679,7 @@
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="3"/>
-        <v>2253.5714285714284</v>
+        <v>2243.5714285714284</v>
       </c>
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
@@ -2752,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="W28" s="1">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="X28" s="1">
         <v>0</v>
@@ -2783,7 +2783,7 @@
       </c>
       <c r="AG28" s="1">
         <f t="shared" si="3"/>
-        <v>2253.5714285714284</v>
+        <v>2243.5714285714284</v>
       </c>
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>
@@ -2858,7 +2858,7 @@
         <v>0</v>
       </c>
       <c r="W29" s="1">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="X29" s="1">
         <v>0</v>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="AG29" s="1">
         <f t="shared" si="3"/>
-        <v>1644.5714285714284</v>
+        <v>1634.5714285714284</v>
       </c>
       <c r="AH29" s="6"/>
       <c r="AI29" s="6"/>
@@ -3378,7 +3378,9 @@
       <c r="V42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="W42" s="1"/>
+      <c r="W42" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="X42" s="1"/>
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
@@ -3456,7 +3458,7 @@
         <v>98</v>
       </c>
       <c r="W43" s="1">
-        <v>0</v>
+        <v>840</v>
       </c>
       <c r="X43" s="1">
         <v>0</v>
@@ -3487,7 +3489,7 @@
       </c>
       <c r="AG43" s="1">
         <f>SUM(B43:AF43)</f>
-        <v>6574</v>
+        <v>7414</v>
       </c>
     </row>
     <row r="44" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3683,7 +3685,7 @@
       </c>
       <c r="W46" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>840</v>
       </c>
       <c r="X46" s="5">
         <f t="shared" si="5"/>
@@ -3723,7 +3725,7 @@
       </c>
       <c r="AG46" s="5">
         <f>SUM(B46:AF46)</f>
-        <v>10421</v>
+        <v>11261</v>
       </c>
     </row>
     <row r="47" spans="1:36" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
meal finished at 23rd March
</commit_message>
<xml_diff>
--- a/Nayem_meal.xlsx
+++ b/Nayem_meal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF2ED56-159D-49F1-B526-548965C611D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D53E76D-A24E-4676-864E-109A992DCFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W44" sqref="W44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3:X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -764,10 +764,10 @@
         <v>2.5</v>
       </c>
       <c r="W3" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="X3" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="Y3" s="1">
         <v>0</v>
@@ -795,19 +795,19 @@
       </c>
       <c r="AG3" s="1">
         <f>SUM(B3:AF3)</f>
-        <v>34.5</v>
+        <v>39.5</v>
       </c>
       <c r="AH3" s="6">
         <f>AG46/AG18</f>
-        <v>36.443365695792878</v>
+        <v>32.735465116279073</v>
       </c>
       <c r="AI3" s="1">
         <f>AG3*AH3</f>
-        <v>1257.2961165048544</v>
+        <v>1293.0508720930234</v>
       </c>
       <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ16" si="0">AG23-AI3</f>
-        <v>-273.7246879334258</v>
+        <v>-309.47944352159482</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>3</v>
@@ -881,10 +881,10 @@
         <v>2.5</v>
       </c>
       <c r="W4" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="X4" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="Y4" s="1">
         <v>0</v>
@@ -912,16 +912,16 @@
       </c>
       <c r="AG4" s="1">
         <f>SUM(B4:AF4)</f>
-        <v>34.5</v>
+        <v>39.5</v>
       </c>
       <c r="AH4" s="6"/>
       <c r="AI4" s="1">
         <f>AG4*AH3</f>
-        <v>1257.2961165048544</v>
+        <v>1293.0508720930234</v>
       </c>
       <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>211.27531206657409</v>
+        <v>175.52055647840507</v>
       </c>
       <c r="AK4" s="2" t="s">
         <v>5</v>
@@ -995,10 +995,10 @@
         <v>2.5</v>
       </c>
       <c r="W5" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="X5" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="Y5" s="1">
         <v>0</v>
@@ -1026,16 +1026,16 @@
       </c>
       <c r="AG5" s="1">
         <f t="shared" ref="AG5:AG16" si="1">SUM(B5:AF5)</f>
-        <v>37.5</v>
+        <v>42.5</v>
       </c>
       <c r="AH5" s="6"/>
       <c r="AI5" s="1">
         <f>AG5*AH3</f>
-        <v>1366.6262135922329</v>
+        <v>1391.2572674418607</v>
       </c>
       <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>366.9452149791955</v>
+        <v>342.31416112956776</v>
       </c>
       <c r="AK5" s="2" t="s">
         <v>15</v>
@@ -1109,10 +1109,10 @@
         <v>1.5</v>
       </c>
       <c r="W6" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="X6" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="Y6" s="1">
         <v>0</v>
@@ -1140,16 +1140,16 @@
       </c>
       <c r="AG6" s="1">
         <f t="shared" si="1"/>
-        <v>49.5</v>
+        <v>54.5</v>
       </c>
       <c r="AH6" s="6"/>
       <c r="AI6" s="1">
         <f>AG6*AH3</f>
-        <v>1803.9466019417475</v>
+        <v>1784.0828488372094</v>
       </c>
       <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>-490.37517337031909</v>
+        <v>-470.511420265781</v>
       </c>
       <c r="AK6" s="2" t="s">
         <v>16</v>
@@ -1223,10 +1223,10 @@
         <v>2.5</v>
       </c>
       <c r="W7" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="X7" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="Y7" s="1">
         <v>0</v>
@@ -1254,16 +1254,16 @@
       </c>
       <c r="AG7" s="1">
         <f t="shared" si="1"/>
-        <v>49.5</v>
+        <v>54.5</v>
       </c>
       <c r="AH7" s="6"/>
       <c r="AI7" s="1">
         <f>AG7*AH3</f>
-        <v>1803.9466019417475</v>
+        <v>1784.0828488372094</v>
       </c>
       <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>439.62482662968091</v>
+        <v>459.488579734219</v>
       </c>
       <c r="AK7" s="2" t="s">
         <v>6</v>
@@ -1337,10 +1337,10 @@
         <v>2.5</v>
       </c>
       <c r="W8" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="X8" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="Y8" s="1">
         <v>0</v>
@@ -1368,16 +1368,16 @@
       </c>
       <c r="AG8" s="1">
         <f t="shared" si="1"/>
-        <v>51.5</v>
+        <v>56.5</v>
       </c>
       <c r="AH8" s="6"/>
       <c r="AI8" s="1">
         <f>AG8*AH3</f>
-        <v>1876.8333333333333</v>
+        <v>1849.5537790697676</v>
       </c>
       <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>366.73809523809518</v>
+        <v>394.0176495016608</v>
       </c>
       <c r="AK8" s="2" t="s">
         <v>4</v>
@@ -1451,10 +1451,10 @@
         <v>2.5</v>
       </c>
       <c r="W9" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="X9" s="1">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="Y9" s="1">
         <v>0</v>
@@ -1482,16 +1482,16 @@
       </c>
       <c r="AG9" s="1">
         <f>SUM(B9:AF9)</f>
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="AH9" s="6"/>
       <c r="AI9" s="1">
         <f>AG9*AH3</f>
-        <v>1895.0550161812296</v>
+        <v>1865.9215116279072</v>
       </c>
       <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>-260.48358760980113</v>
+        <v>-231.35008305647875</v>
       </c>
       <c r="AK9" s="2" t="s">
         <v>17</v>
@@ -1921,11 +1921,11 @@
       </c>
       <c r="W17" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="X17" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>17.5</v>
       </c>
       <c r="Y17" s="1">
         <f t="shared" si="2"/>
@@ -2001,7 +2001,7 @@
       <c r="AF18" s="7"/>
       <c r="AG18" s="1">
         <f>SUM(AG3:AG16)</f>
-        <v>309</v>
+        <v>344</v>
       </c>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>

</xml_diff>